<commit_message>
Regularize some columns according to SSSOM standards - see https://mapping-commons.github.io/sssom/spec/#tsv https://mapping-commons.github.io/sssom/Mapping/#slots
</commit_message>
<xml_diff>
--- a/crosswalks/MarineCoastal-IUCNGET/MarineCoastal-IUCNGET.xlsx
+++ b/crosswalks/MarineCoastal-IUCNGET/MarineCoastal-IUCNGET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\MarineCoastal-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\MarineCoastal-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A4EBF2-A4D5-49D9-B5EC-D51AAD001A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C3BC25-0D9F-42DC-8C44-309A9883B608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="6240" yWindow="7065" windowWidth="29595" windowHeight="16200" activeTab="2" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="IUCN GET L3" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,21 @@
     <sheet name="Crosswalk_V2" sheetId="3" r:id="rId3"/>
     <sheet name="SSSOM" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -35,19 +46,28 @@
   <commentList>
     <comment ref="A30" authorId="0" shapeId="0" xr:uid="{448C10AB-2548-445D-8D1C-94025C8E7CB6}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Should this be Marine?</t>
-        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={61E97ACF-2248-410F-BA66-E912F5FD73E7}</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{61E97ACF-2248-410F-BA66-E912F5FD73E7}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Is this actually the mapping author? </t>
       </text>
     </comment>
   </commentList>
@@ -55,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="348">
   <si>
     <t>Realm</t>
   </si>
@@ -1128,10 +1148,16 @@
     <t>https://orcid.org/0000-0003-4254-8683</t>
   </si>
   <si>
-    <t>Reviewer1_notes</t>
-  </si>
-  <si>
     <t>Piers Dunstan</t>
+  </si>
+  <si>
+    <t>reviewer_id</t>
+  </si>
+  <si>
+    <t>orcid:0000-0002-2568-5945</t>
+  </si>
+  <si>
+    <t>reviewer_label</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,6 +1254,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1360,14 +1392,15 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Simon Cox" id="{79658783-6508-45FB-8D3F-D9B797DAE8A5}" userId="fcabc4d7e599448e" providerId="Windows Live"/>
   <person displayName="Macfarlane, Craig (Environment, Floreat)" id="{56E0A7AD-2F67-4F51-9367-6370C1F6A9AE}" userId="S::mac508@csiro.au::44651e22-f133-4a68-8459-bbcd09b63482" providerId="AD"/>
 </personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1405,7 +1438,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1511,7 +1544,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1653,7 +1686,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1669,8 +1702,8 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2023-12-13T01:54:45.53" personId="{56E0A7AD-2F67-4F51-9367-6370C1F6A9AE}" id="{8380B0E1-4B86-47DC-B961-EFC84422D541}">
-    <text>I'm not sure what these numbers mean.  The classes in Appendix A of the Dunstan et al. 2022 go up to 18.</text>
+  <threadedComment ref="G1" dT="2024-01-16T02:50:12.04" personId="{79658783-6508-45FB-8D3F-D9B797DAE8A5}" id="{61E97ACF-2248-410F-BA66-E912F5FD73E7}">
+    <text xml:space="preserve">Is this actually the mapping author? </text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1683,16 +1716,16 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="43.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.81640625" customWidth="1"/>
-    <col min="10" max="10" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>95</v>
       </c>
@@ -1753,7 +1786,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>95</v>
       </c>
@@ -1782,7 +1815,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>95</v>
       </c>
@@ -1811,7 +1844,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>95</v>
       </c>
@@ -1840,7 +1873,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>95</v>
       </c>
@@ -1870,7 +1903,7 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>95</v>
       </c>
@@ -1900,7 +1933,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>95</v>
       </c>
@@ -1930,7 +1963,7 @@
       </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>95</v>
       </c>
@@ -1959,7 +1992,7 @@
         <v>43980.494606481479</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>95</v>
       </c>
@@ -1988,7 +2021,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>95</v>
       </c>
@@ -2017,7 +2050,7 @@
         <v>44741.270972222221</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>153</v>
       </c>
@@ -2046,7 +2079,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>153</v>
       </c>
@@ -2075,7 +2108,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>153</v>
       </c>
@@ -2104,7 +2137,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>153</v>
       </c>
@@ -2133,7 +2166,7 @@
         <v>44383.104687500003</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>153</v>
       </c>
@@ -2165,7 +2198,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>184</v>
       </c>
@@ -2194,7 +2227,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>184</v>
       </c>
@@ -2223,7 +2256,7 @@
         <v>43980.49559027778</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>184</v>
       </c>
@@ -2252,7 +2285,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>184</v>
       </c>
@@ -2281,7 +2314,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>184</v>
       </c>
@@ -2316,7 +2349,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>184</v>
       </c>
@@ -2348,7 +2381,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>184</v>
       </c>
@@ -2380,7 +2413,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>228</v>
       </c>
@@ -2415,7 +2448,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>228</v>
       </c>
@@ -2447,7 +2480,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>242</v>
       </c>
@@ -2479,7 +2512,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>242</v>
       </c>
@@ -2508,7 +2541,7 @@
         <v>43850.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>242</v>
       </c>
@@ -2537,7 +2570,7 @@
         <v>44041.421215277784</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>262</v>
       </c>
@@ -2569,7 +2602,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>262</v>
       </c>
@@ -2601,7 +2634,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>262</v>
       </c>
@@ -2633,7 +2666,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>262</v>
       </c>
@@ -2665,7 +2698,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>291</v>
       </c>
@@ -2697,7 +2730,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>291</v>
       </c>
@@ -2729,7 +2762,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>305</v>
       </c>
@@ -2775,17 +2808,17 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="121.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.26953125" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2811,7 +2844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2837,7 +2870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2863,7 +2896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2889,7 +2922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2916,7 +2949,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2943,7 +2976,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2969,7 +3002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -2995,7 +3028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3021,7 +3054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3047,7 +3080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -3073,7 +3106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -3099,7 +3132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -3125,7 +3158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -3151,7 +3184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -3177,7 +3210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -3203,7 +3236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -3229,7 +3262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -3255,7 +3288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -3281,7 +3314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -3307,7 +3340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -3333,7 +3366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -3359,7 +3392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -3385,7 +3418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -3411,7 +3444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -3437,7 +3470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -3463,7 +3496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -3480,7 +3513,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
@@ -3497,7 +3530,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
@@ -3514,7 +3547,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>73</v>
       </c>
@@ -3539,43 +3572,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869F0E0B-08B8-4651-AFE7-4266EA9CC8AA}">
-  <dimension ref="A1:G38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869F0E0B-08B8-4651-AFE7-4266EA9CC8AA}">
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
-    <col min="4" max="4" width="34.26953125" customWidth="1"/>
-    <col min="5" max="5" width="40.26953125" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="6" width="40.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>330</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" t="s">
+        <v>321</v>
+      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>322</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>347</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>337</v>
       </c>
@@ -3587,10 +3628,13 @@
         <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>337</v>
       </c>
@@ -3602,10 +3646,13 @@
         <v>131</v>
       </c>
       <c r="F3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>337</v>
       </c>
@@ -3617,10 +3664,13 @@
         <v>136</v>
       </c>
       <c r="F4" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>337</v>
       </c>
@@ -3632,13 +3682,16 @@
         <v>147</v>
       </c>
       <c r="F5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G5" t="s">
+        <v>344</v>
+      </c>
+      <c r="H5" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>337</v>
       </c>
@@ -3650,10 +3703,13 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>337</v>
       </c>
@@ -3665,10 +3721,13 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G7" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>337</v>
       </c>
@@ -3680,10 +3739,13 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>337</v>
       </c>
@@ -3695,10 +3757,13 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G9" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>337</v>
       </c>
@@ -3710,10 +3775,13 @@
         <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G10" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>337</v>
       </c>
@@ -3725,10 +3793,13 @@
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>337</v>
       </c>
@@ -3740,10 +3811,13 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>337</v>
       </c>
@@ -3755,10 +3829,13 @@
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G13" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>337</v>
       </c>
@@ -3770,10 +3847,13 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>337</v>
       </c>
@@ -3785,10 +3865,13 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>337</v>
       </c>
@@ -3800,10 +3883,13 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G16" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>337</v>
       </c>
@@ -3815,10 +3901,13 @@
         <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G17" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>337</v>
       </c>
@@ -3830,13 +3919,16 @@
         <v>112</v>
       </c>
       <c r="F18" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G18" t="s">
+        <v>344</v>
+      </c>
+      <c r="H18" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>337</v>
       </c>
@@ -3848,10 +3940,13 @@
         <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G19" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>337</v>
       </c>
@@ -3863,10 +3958,13 @@
         <v>49</v>
       </c>
       <c r="F20" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G20" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>337</v>
       </c>
@@ -3878,10 +3976,13 @@
         <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G21" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>337</v>
       </c>
@@ -3893,10 +3994,13 @@
         <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G22" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>337</v>
       </c>
@@ -3908,10 +4012,13 @@
         <v>49</v>
       </c>
       <c r="F23" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>337</v>
       </c>
@@ -3923,10 +4030,13 @@
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G24" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>337</v>
       </c>
@@ -3938,10 +4048,13 @@
         <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G25" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>337</v>
       </c>
@@ -3953,10 +4066,13 @@
         <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G26" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>338</v>
       </c>
@@ -3968,10 +4084,13 @@
         <v>63</v>
       </c>
       <c r="F27" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G27" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>338</v>
       </c>
@@ -3982,10 +4101,13 @@
         <v>63</v>
       </c>
       <c r="F28" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G28" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>338</v>
       </c>
@@ -3996,10 +4118,13 @@
         <v>69</v>
       </c>
       <c r="F29" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G29" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>338</v>
       </c>
@@ -4010,10 +4135,13 @@
         <v>167</v>
       </c>
       <c r="F30" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G30" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>338</v>
       </c>
@@ -4024,13 +4152,16 @@
         <v>173</v>
       </c>
       <c r="F31" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G31" t="s">
+        <v>344</v>
+      </c>
+      <c r="H31" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>331</v>
       </c>
@@ -4041,10 +4172,13 @@
         <v>76</v>
       </c>
       <c r="F32" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G32" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>331</v>
       </c>
@@ -4055,10 +4189,13 @@
         <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G33" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>331</v>
       </c>
@@ -4069,10 +4206,13 @@
         <v>82</v>
       </c>
       <c r="F34" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G34" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>331</v>
       </c>
@@ -4083,22 +4223,27 @@
         <v>85</v>
       </c>
       <c r="F35" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+      <c r="G35" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E38" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F38" t="s">
-        <v>345</v>
-      </c>
+      <c r="F38" s="5"/>
       <c r="G38" t="s">
+        <v>344</v>
+      </c>
+      <c r="H38" t="s">
         <v>317</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4110,25 +4255,25 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>318</v>
       </c>
@@ -4172,7 +4317,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE(Crosswalk_V2!A2,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B2," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shelf-unvegetated-sediments</v>
@@ -4211,7 +4356,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE(Crosswalk_V2!A3,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shelf-unvegetated-sediments</v>
@@ -4250,7 +4395,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE(Crosswalk_V2!A4,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B4," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shelf-unvegetated-sediments</v>
@@ -4289,7 +4434,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE(Crosswalk_V2!A5,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B5," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shelf-unvegetated-sediments</v>
@@ -4328,7 +4473,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CONCATENATE(Crosswalk_V2!A6,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B6," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Upper-slope-sediments</v>
@@ -4364,7 +4509,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CONCATENATE(Crosswalk_V2!A7,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B7," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Mid-slope-sediments</v>
@@ -4400,7 +4545,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CONCATENATE(Crosswalk_V2!A8,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B8," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Lower-slope-reef-&amp;-sediments</v>
@@ -4436,7 +4581,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CONCATENATE(Crosswalk_V2!A9,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B9," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Abyss-reefs-&amp;-sediments</v>
@@ -4472,7 +4617,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE(Crosswalk_V2!A10,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B10," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Seamount-sediments</v>
@@ -4508,7 +4653,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CONCATENATE(Crosswalk_V2!A11,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B11," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Seamount-reefs</v>
@@ -4544,7 +4689,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CONCATENATE(Crosswalk_V2!A12,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B12," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shelf-incising-canyons</v>
@@ -4580,7 +4725,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CONCATENATE(Crosswalk_V2!A13,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B13," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shelf-vegetated-sediments</v>
@@ -4616,7 +4761,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>CONCATENATE(Crosswalk_V2!A14,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B14," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Oceanic-coral-reefs</v>
@@ -4652,7 +4797,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>CONCATENATE(Crosswalk_V2!A15,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B15," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Oceanic-corals-reefs</v>
@@ -4688,7 +4833,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>CONCATENATE(Crosswalk_V2!A16,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Oceanic-shallow-coral-reefs</v>
@@ -4724,7 +4869,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>CONCATENATE(Crosswalk_V2!A17,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B17," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shallow-rocky-reefs</v>
@@ -4760,7 +4905,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>CONCATENATE(Crosswalk_V2!A18,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B18," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shallow-rocky-reefs</v>
@@ -4796,7 +4941,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>CONCATENATE(Crosswalk_V2!A19,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B19," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Shallow-rocky-reefs</v>
@@ -4832,7 +4977,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>CONCATENATE(Crosswalk_V2!A20,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Mesophotic-coral-reefs</v>
@@ -4868,7 +5013,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>CONCATENATE(Crosswalk_V2!A21,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B21," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Mesophotic-rocky-reefs</v>
@@ -4904,7 +5049,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>CONCATENATE(Crosswalk_V2!A22,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B22," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Oceanic-mesophotic-coral-reefs</v>
@@ -4940,7 +5085,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>CONCATENATE(Crosswalk_V2!A23,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B23," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Rariphotic-shelf-reefs</v>
@@ -4976,7 +5121,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>CONCATENATE(Crosswalk_V2!A24,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B24," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Upper-slope-reefs</v>
@@ -5012,7 +5157,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>CONCATENATE(Crosswalk_V2!A25,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B25," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Upper-slope-reefs</v>
@@ -5048,7 +5193,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>CONCATENATE(Crosswalk_V2!A26,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B26," - ","")," ","-"),"/","-or-"))</f>
         <v>benthic:Mid-slope-reefs</v>
@@ -5084,7 +5229,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>CONCATENATE(Crosswalk_V2!A27,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B27," - ","")," ","-"),"/","-or-"))</f>
         <v>pelagic:On-shelf-(neritic)-epipelagic</v>
@@ -5120,7 +5265,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>CONCATENATE(Crosswalk_V2!A28,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B28," - ","")," ","-"),"/","-or-"))</f>
         <v>pelagic:Off-shelf-(oceanic)-epipelagic</v>
@@ -5156,7 +5301,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>CONCATENATE(Crosswalk_V2!A29,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B29," - ","")," ","-"),"/","-or-"))</f>
         <v>pelagic:Mesopelagic</v>
@@ -5192,7 +5337,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>CONCATENATE(Crosswalk_V2!A30,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B30," - ","")," ","-"),"/","-or-"))</f>
         <v>pelagic:Bathypelagic-&amp;-Abyssopelagic</v>
@@ -5231,7 +5376,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>CONCATENATE(Crosswalk_V2!A31,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B31," - ","")," ","-"),"/","-or-"))</f>
         <v>pelagic:Bathypelagic-&amp;-Abyssopelagic</v>
@@ -5270,7 +5415,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>CONCATENATE(Crosswalk_V2!A32,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B32," - ","")," ","-"),"/","-or-"))</f>
         <v>coastal:Saltmarsh</v>
@@ -5306,7 +5451,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>CONCATENATE(Crosswalk_V2!A33,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B33," - ","")," ","-"),"/","-or-"))</f>
         <v>coastal:Intertidal-seagrass</v>
@@ -5342,7 +5487,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>CONCATENATE(Crosswalk_V2!A34,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B34," - ","")," ","-"),"/","-or-"))</f>
         <v>coastal:Mangroves</v>
@@ -5378,7 +5523,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>CONCATENATE(Crosswalk_V2!A35,":",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B35," - ","")," ","-"),"/","-or-"))</f>
         <v>coastal:Kelp</v>
@@ -5425,32 +5570,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -5726,6 +5845,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -5777,25 +5922,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5814,6 +5940,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
   <ds:schemaRefs>

</xml_diff>